<commit_message>
recorrect classification accracy of SD on Beef
</commit_message>
<xml_diff>
--- a/result/results of Classification Accuracy.xlsx
+++ b/result/results of Classification Accuracy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>ST</t>
   </si>
@@ -22,76 +22,58 @@
     <t>LS</t>
   </si>
   <si>
+    <t>SALSA-R</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>Adiac</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>ChlorineConcentration</t>
+  </si>
+  <si>
+    <t>DiatomSizeReduction</t>
+  </si>
+  <si>
+    <t>ItalyPowerDemand</t>
+  </si>
+  <si>
+    <t>Lightning7</t>
+  </si>
+  <si>
+    <t>MedicalImages</t>
+  </si>
+  <si>
+    <t>MoteStrain</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>TwoLeadECG</t>
+  </si>
+  <si>
     <t>FSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>gRSF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SALSA-R</t>
   </si>
   <si>
     <t>SD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FS</t>
   </si>
   <si>
     <t>RS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adiac</t>
-  </si>
-  <si>
-    <t>Beef</t>
-  </si>
-  <si>
-    <t>ChlorineConcentration</t>
   </si>
   <si>
     <t>Coffee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DiatomSizeReduction</t>
-  </si>
-  <si>
-    <t>ItalyPowerDemand</t>
-  </si>
-  <si>
-    <t>Lightning7</t>
-  </si>
-  <si>
-    <t>MedicalImages</t>
-  </si>
-  <si>
-    <t>MoteStrain</t>
   </si>
   <si>
     <t>Symbols</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trace</t>
-  </si>
-  <si>
-    <t>TwoLeadECG</t>
-  </si>
-  <si>
-    <t>FSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gRSF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -458,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -479,48 +461,48 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.78260869600000005</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="C2" s="1">
-        <v>0.52173913043478204</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="D2" s="1">
-        <v>0.78516624040920702</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="E2" s="1">
-        <v>0.73150000000000004</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="F2" s="1">
-        <v>0.72570000000000001</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="G2" s="1">
         <v>0.58299999999999996</v>
       </c>
       <c r="H2" s="1">
-        <v>0.59335000000000004</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="I2" s="1">
         <v>0.51600000000000001</v>
@@ -546,28 +528,28 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>0.9</v>
       </c>
       <c r="C3" s="1">
-        <v>0.86666666666666603</v>
+        <v>0.86699999999999999</v>
       </c>
       <c r="D3" s="1">
-        <v>0.83333333333333304</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="E3" s="1">
-        <v>0.63329999999999997</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F3" s="1">
-        <v>0.6089</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="G3" s="1">
-        <v>0.97499999999999998</v>
+        <v>0.50700000000000001</v>
       </c>
       <c r="H3" s="1">
-        <v>0.56666700000000003</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="I3" s="1">
         <v>0.32400000000000001</v>
@@ -593,28 +575,28 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.69973958300000005</v>
+        <v>0.7</v>
       </c>
       <c r="C4" s="1">
-        <v>0.59244791666666596</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="D4" s="1">
-        <v>0.64322916666666596</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="E4" s="1">
-        <v>0.65780000000000005</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="F4" s="1">
-        <v>0.67110000000000003</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="G4" s="1">
         <v>0.55300000000000005</v>
       </c>
       <c r="H4" s="1">
-        <v>0.54635400000000001</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="I4" s="1">
         <v>0.57199999999999995</v>
@@ -640,10 +622,10 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
-        <v>0.96428571399999996</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -652,16 +634,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0.96430000000000005</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="F5" s="1">
-        <v>0.95950000000000002</v>
+        <v>0.96</v>
       </c>
       <c r="G5" s="1">
         <v>0.96099999999999997</v>
       </c>
       <c r="H5" s="1">
-        <v>0.92857100000000004</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="I5" s="1">
         <v>0.76900000000000002</v>
@@ -687,28 +669,28 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>0.92483660099999998</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="C6" s="1">
-        <v>0.98039215686274495</v>
+        <v>0.98</v>
       </c>
       <c r="D6" s="1">
-        <v>0.85620915032679701</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="E6" s="1">
-        <v>0.77880000000000005</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="F6" s="1">
-        <v>0.76919999999999999</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="G6" s="1">
         <v>0.89600000000000002</v>
       </c>
       <c r="H6" s="1">
-        <v>0.86601300000000003</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="I6" s="1">
         <v>0.77400000000000002</v>
@@ -734,28 +716,28 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>0.94752186599999999</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="C7" s="1">
-        <v>0.96015549076773499</v>
+        <v>0.96</v>
       </c>
       <c r="D7" s="1">
-        <v>0.93974732750242895</v>
+        <v>0.94</v>
       </c>
       <c r="E7" s="1">
-        <v>0.94359999999999999</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="F7" s="1">
-        <v>0.95120000000000005</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="G7" s="1">
         <v>0.92</v>
       </c>
       <c r="H7" s="1">
-        <v>0.91739599999999999</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="I7" s="1">
         <v>0.92400000000000004</v>
@@ -781,16 +763,16 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>0.72602739699999996</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="C8" s="1">
-        <v>0.79452054794520499</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="D8" s="1">
-        <v>0.73972602739726001</v>
+        <v>0.74</v>
       </c>
       <c r="E8" s="1">
         <v>0.72599999999999998</v>
@@ -802,7 +784,7 @@
         <v>0.65200000000000002</v>
       </c>
       <c r="H8" s="1">
-        <v>0.64383599999999996</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="I8" s="1">
         <v>0.63500000000000001</v>
@@ -828,28 +810,28 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>0.66973684200000005</v>
+        <v>0.67</v>
       </c>
       <c r="C9" s="1">
-        <v>0.66447368421052599</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="D9" s="1">
-        <v>0.71184210526315705</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E9" s="1">
-        <v>0.69740000000000002</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F9" s="1">
-        <v>0.6855</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="G9" s="1">
         <v>0.67600000000000005</v>
       </c>
       <c r="H9" s="1">
-        <v>0.62368400000000002</v>
+        <v>0.624</v>
       </c>
       <c r="I9" s="1">
         <v>0.52900000000000003</v>
@@ -875,28 +857,28 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>0.89696485599999998</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="C10" s="1">
-        <v>0.88338658146964799</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>0.89456869009584605</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="E10" s="1">
-        <v>0.95209999999999995</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="F10" s="1">
-        <v>0.85409999999999997</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="G10" s="1">
         <v>0.78300000000000003</v>
       </c>
       <c r="H10" s="1">
-        <v>0.77715699999999999</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="I10" s="1">
         <v>0.81499999999999995</v>
@@ -922,28 +904,28 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
-        <v>0.88241206000000005</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>0.93165829145728596</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="D11" s="1">
-        <v>0.95075376884422103</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="E11" s="1">
-        <v>0.75470000000000004</v>
+        <v>0.755</v>
       </c>
       <c r="F11" s="1">
-        <v>0.86350000000000005</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="G11" s="1">
         <v>0.86499999999999999</v>
       </c>
       <c r="H11" s="1">
-        <v>0.93366800000000005</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="I11" s="1">
         <v>0.79500000000000004</v>
@@ -969,7 +951,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -984,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>0.99970000000000003</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <v>0.96499999999999997</v>
@@ -1016,28 +998,28 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>0.99736611100000006</v>
+        <v>0.997</v>
       </c>
       <c r="C13" s="1">
-        <v>0.99648814749780501</v>
+        <v>0.996</v>
       </c>
       <c r="D13" s="1">
-        <v>0.98595258999122004</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="E13" s="1">
-        <v>0.99119999999999997</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="F13" s="1">
-        <v>0.95779999999999998</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="G13" s="1">
         <v>0.86699999999999999</v>
       </c>
       <c r="H13" s="1">
-        <v>0.92449499999999996</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="I13" s="1">
         <v>0.91400000000000003</v>
@@ -1063,36 +1045,28 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.15">
       <c r="B14" s="3">
-        <f t="shared" ref="B14:I14" si="0">AVERAGE(B2:B13)</f>
-        <v>0.86595831050000005</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.84932738449825529</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.86171069998584471</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.81922499999999998</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.81176666666666686</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.80800000000000016</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.77676591666666672</v>
+        <v>0.77700000000000002</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.70841666666666681</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1141,27 +1115,27 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -1190,28 +1164,28 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>3</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>4</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2">
         <v>6</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>7</v>
       </c>
       <c r="I21" s="2">
         <v>8</v>
@@ -1219,7 +1193,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
@@ -1256,7 +1230,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2">
         <v>3.5</v>
@@ -1285,7 +1259,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
@@ -1314,7 +1288,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
@@ -1351,7 +1325,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
         <v>2.5</v>
@@ -1388,7 +1362,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2">
         <v>5</v>
@@ -1425,7 +1399,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2">
         <v>2</v>
@@ -1462,7 +1436,7 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2">
         <v>4</v>
@@ -1499,7 +1473,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2">
         <v>3.5</v>
@@ -1536,7 +1510,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B31" s="2">
         <v>1</v>
@@ -1573,35 +1547,27 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B32" s="4">
-        <f t="shared" ref="B32:I32" si="1">AVERAGE(B20:B31)</f>
-        <v>2.625</v>
+        <v>2.5419999999999998</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="1"/>
-        <v>3.1666666666666665</v>
+        <v>3.0830000000000002</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="1"/>
-        <v>3.0833333333333335</v>
+        <v>3</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="1"/>
-        <v>3.7083333333333335</v>
+        <v>3.625</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="1"/>
-        <v>4.625</v>
+        <v>4.5419999999999998</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="1"/>
-        <v>5.583333333333333</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="1"/>
-        <v>5.958333333333333</v>
+        <v>5.875</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="N32" s="2"/>

</xml_diff>